<commit_message>
Refine code and enhance documentation
</commit_message>
<xml_diff>
--- a/categories.xlsx
+++ b/categories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tswar/PycharmProjects/ra-repo-parser/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toufikswar/Documents/dev/waitress-salesforce/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D20D2A7-C352-CD40-944B-482230B832B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B277A2FE-9B24-454F-9CAB-A80F834B278A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-10620" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_remote_actions" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="475">
   <si>
     <t>Name</t>
   </si>
@@ -1067,6 +1067,399 @@
   </si>
   <si>
     <t>https://www.nexthink.com/library/firefox-browser-management/#get-firefox-plugins</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-update/#install-windows-update</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-update/#get-last-feature-update-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-update/#get-windows-feature-update-diagnosis</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-update/#invoke-windows-update</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/green-it/#get-battery-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/green-it/#set-power-plan</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/green-it/#get-user-folder-size</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/green-it/#get-power-plan</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/green-it/#get-consumption-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/network-drives/#get-network-drives</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/network-drives/#map-network-drive</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/azure-ad-registration-check/#get-device-azure-ad-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-11-readiness/#get-secure-boot-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-11-readiness/#get-directx-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-11-readiness/#get-bitlocker-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/network-management/#get-network-configuration</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/network-management/#get-wi-fi-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/network-management/#test-connection-from-device</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/network-management/#clear-dns-cache</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/network-management/#get-interface-connection-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/network-management/#get-active-ip-address</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/microsoft-edge/#get-microsoft-edge-plugins</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/microsoft-edge/#set-microsoft-edge-plugins</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/microsoft-edge/#clear-microsoft-edge-settings</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/internet-explorer/#clear-internet-explorer-11-settings</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/internet-explorer/#get-internet-explorer-plugins</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/internet-explorer/#set-internet-explorer-plugins</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/officescan-management/#start-officescan-location-scan</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/officescan-management/#update-officescan-definition</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/jamf-management/#reinstall-jamf</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/jamf-management/#get-jamf-agent-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/jamf-management/#invoke-jamf-reconnect</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/application-auto-start-impact/#get-startup-impact</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/application-auto-start-impact/#disable-application-from-startup-menu</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/chatbot-content-pack/#get-gpo-startup-impact</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/chatbot-content-pack/#disk-cleanup</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/chatbot-content-pack/#system-cleanup</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/chatbot-content-pack/#request-vpn-connection-for-compliance</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/chatbot-content-pack/#update-group-policy-settings</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/chatbot-content-pack/#get-hardware-and-bios-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/chatbot-content-pack/#reset-print-spooler</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/chatbot-content-pack/#skype-for-business-diagnostics</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/chatbot-content-pack/#get-windows-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/macos-ensure-compliance-state/#get-accounts-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/macos-ensure-compliance-state/#get-auto-login-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/macos-ensure-compliance-state/#get-automatic-updates-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/macos-ensure-compliance-state/#get-encryption-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/macos-ensure-compliance-state/#get-firewall-options</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/macos-ensure-compliance-state/#get-xprotect-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/automate-device-restart-logoff-shutdown-windows-library-pack/#invoke-log-off-for-windows</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/automate-device-restart-logoff-shutdown-windows-library-pack/#invoke-shut-down-for-windows</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/automate-device-restart-logoff-shutdown-windows-library-pack/#restart-windows-device</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/automate-device-restart-logoff-shutdown-macos-library-pack/#invoke-log-off-for-macos</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/automate-device-restart-logoff-shutdown-macos-library-pack/#invoke-shut-down-for-macos</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/automate-device-restart-logoff-shutdown-macos-library-pack/#restart-macos-device</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-service-information/#restart-service</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-service-information/#get-service-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-service-information/#set-service-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/device-compliance-advanced/#hosts-file-integrity-check</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/device-compliance-advanced/#get-smb1-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/device-compliance-advanced/#disable-smb1</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/device-compliance-advanced/#remove-certificates</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/device-compliance-advanced/#trusted-root-certification-authorities-certificate-store-integrity-check</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/device-compliance-advanced/#get-windows-security-center-health-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-registry/#get-windows-registry-key-values</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-registry/#set-windows-registry-key-value</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-defender-management/#get-windows-defender-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-defender-management/#update-windows-defender-definition</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-defender-management/#set-windows-defender-scheduled-scan</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-defender-management/#start-windows-defender-scan</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/microsoft-visio-and-project-management/#uninstall-microsoft-office-visio-and-project</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/software-asset-optimization/#uninstall-adobe-dc-professional</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/user-access-control/#get-local-administrators</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/user-access-control/#enable-user-access-control</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-11-migration/#invoke-sccm-upgrade-to-windows-11</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/geolocation/#get-geolocation</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/user-login-management/#kerberos-password-expiration-reminder</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/citrix-management/#get-virtual-apps-session-response-time</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/user-login-management/#remove-credentials-from-credential-manager</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/event-logs/#get-event-log</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/event-logs/#get-number-of-log-events</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/return-to-the-office-readiness/#get-computer-assigned-group-policy</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/return-to-the-office-readiness/#test-domain-connection</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/cisco-anyconnect/#check-anyconnect-timeout</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/hardware-asset-renewal-advanced/#get-disk-health</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-information/#get-frameworks-version</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/performance-monitor-management/#get-performance-monitor-data</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/engage-accessibility/#enable-tray-accessibility</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/hardware-and-bios-information/#get-physical-disks-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/apple-unified-logging/#get-apple-unified-logging</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/green-it/#get-onedrive-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-information/#read-mini-dump</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/disk-cleanup/#clear-recycle-bin</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/virtualization-avd-advanced/#get-azure-virtual-desktop-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/mcafee-management/#get-mcafee-agent-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/mcafee-management/#update-mcafee-agent-policy</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/user-login-management/#get-failed-logins</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/manage-configuration-drift/#get-configuration-drift</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/mitigate-cve20191552/#mitigate-cve20191552</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/citrix-management/#get-citrix-vdi-connection-details</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-information/#get-powershell-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/vulnerability-management/#update-winrar</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/employee-self-service/#invoke-proactive-password-reset</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/device-network-isolation/#disable-device-network-isolation</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/device-network-isolation/#enable-device-network-isolation</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/application-experience-configure-browser-extension/#set-application-experience</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-information/#get-device-manager-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-information/#get-folder-size</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-information/#get-windows-experience-index</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/disk-encryption/#enable-bitlocker-encryption</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/intune-health/#get-device-hardware-id</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/microsoft-endpoint-manager-remote-actions/#start-application-or-task-sequence</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/microsoft-endpoint-manager-remote-actions/#repair-wmi</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-boot-information/#get-boot-details</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/citrix-management/#get-citrix-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/skype-management/#get-skype-last-call</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/skype-management/#copy-skype-log-files</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/citrix-management/#get-citrix-session-client-versions</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-boot-information/#set-boot-autologger</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/usb-storage-management/#set-usb-storage-access</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/disk-cleanup/#get-old-files-size</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/hardware-and-bios-information/#get-windows-disk-configuration</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/disk-cleanup/#get-file-extension-total-size</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/macos-plist-settings/#get-plist-file-settings</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/windows-management-instrumentation/#get-wmi-data</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/intune-health/#get-microsoft-intune-device-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/hardware-asset-renewal-advanced/#get-warranty-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/usb-audio-device-information/#get-usb-audio-device-information</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/battery-status/#get-multiple-batteries-status</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/hybrid-working-experience/#check-certificate-validity</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/get-application-experience-browser-extension-status/#get-application-experience-browser-extension-status</t>
   </si>
 </sst>
 </file>
@@ -1444,14 +1837,14 @@
   <dimension ref="A1:D246"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="54.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="108.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1620,6 +2013,9 @@
       <c r="C13" t="s">
         <v>261</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>418</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1645,7 +2041,9 @@
       <c r="C15" t="s">
         <v>272</v>
       </c>
-      <c r="D15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1727,6 +2125,9 @@
       <c r="C21" t="s">
         <v>256</v>
       </c>
+      <c r="D21" s="2" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1752,6 +2153,9 @@
       <c r="C23" t="s">
         <v>256</v>
       </c>
+      <c r="D23" s="2" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -1774,6 +2178,9 @@
       <c r="C25" t="s">
         <v>256</v>
       </c>
+      <c r="D25" s="2" t="s">
+        <v>376</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -1785,6 +2192,9 @@
       <c r="C26" t="s">
         <v>250</v>
       </c>
+      <c r="D26" s="2" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -1796,6 +2206,9 @@
       <c r="C27" t="s">
         <v>267</v>
       </c>
+      <c r="D27" s="2" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -1807,6 +2220,9 @@
       <c r="C28" t="s">
         <v>256</v>
       </c>
+      <c r="D28" s="2" t="s">
+        <v>357</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -1818,6 +2234,9 @@
       <c r="C29" t="s">
         <v>256</v>
       </c>
+      <c r="D29" s="2" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -1829,6 +2248,9 @@
       <c r="C30" t="s">
         <v>251</v>
       </c>
+      <c r="D30" s="2" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -1840,6 +2262,9 @@
       <c r="C31" t="s">
         <v>256</v>
       </c>
+      <c r="D31" s="2" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -1851,6 +2276,9 @@
       <c r="C32" t="s">
         <v>271</v>
       </c>
+      <c r="D32" s="2" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -1887,6 +2315,9 @@
       <c r="C35" t="s">
         <v>270</v>
       </c>
+      <c r="D35" s="2" t="s">
+        <v>415</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -1898,6 +2329,9 @@
       <c r="C36" t="s">
         <v>251</v>
       </c>
+      <c r="D36" s="2" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -1923,6 +2357,9 @@
       <c r="C38" t="s">
         <v>256</v>
       </c>
+      <c r="D38" s="2" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
@@ -1934,7 +2371,7 @@
       <c r="C39" t="s">
         <v>256</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="2" t="s">
         <v>286</v>
       </c>
     </row>
@@ -1987,6 +2424,9 @@
       <c r="C43" t="s">
         <v>257</v>
       </c>
+      <c r="D43" s="2" t="s">
+        <v>374</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -1998,6 +2438,9 @@
       <c r="C44" t="s">
         <v>251</v>
       </c>
+      <c r="D44" s="2" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
@@ -2009,6 +2452,9 @@
       <c r="C45" t="s">
         <v>258</v>
       </c>
+      <c r="D45" s="2" t="s">
+        <v>420</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
@@ -2020,6 +2466,9 @@
       <c r="C46" t="s">
         <v>272</v>
       </c>
+      <c r="D46" s="2" t="s">
+        <v>421</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
@@ -2031,6 +2480,9 @@
       <c r="C47" t="s">
         <v>256</v>
       </c>
+      <c r="D47" s="2" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
@@ -2042,6 +2494,9 @@
       <c r="C48" t="s">
         <v>258</v>
       </c>
+      <c r="D48" s="2" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
@@ -2078,6 +2533,9 @@
       <c r="C51" t="s">
         <v>256</v>
       </c>
+      <c r="D51" s="2" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
@@ -2089,6 +2547,9 @@
       <c r="C52" t="s">
         <v>249</v>
       </c>
+      <c r="D52" s="2" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
@@ -2114,6 +2575,9 @@
       <c r="C54" t="s">
         <v>255</v>
       </c>
+      <c r="D54" s="2" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
@@ -2136,6 +2600,9 @@
       <c r="C56" t="s">
         <v>256</v>
       </c>
+      <c r="D56" s="2" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
@@ -2147,6 +2614,9 @@
       <c r="C57" t="s">
         <v>2</v>
       </c>
+      <c r="D57" s="2" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
@@ -2172,6 +2642,9 @@
       <c r="C59" t="s">
         <v>251</v>
       </c>
+      <c r="D59" s="2" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
@@ -2183,6 +2656,9 @@
       <c r="C60" t="s">
         <v>272</v>
       </c>
+      <c r="D60" s="2" t="s">
+        <v>425</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
@@ -2194,6 +2670,9 @@
       <c r="C61" t="s">
         <v>256</v>
       </c>
+      <c r="D61" s="2" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
@@ -2205,6 +2684,9 @@
       <c r="C62" t="s">
         <v>256</v>
       </c>
+      <c r="D62" s="2" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -2216,6 +2698,9 @@
       <c r="C63" t="s">
         <v>250</v>
       </c>
+      <c r="D63" s="2" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
@@ -2255,6 +2740,9 @@
       <c r="C66" t="s">
         <v>256</v>
       </c>
+      <c r="D66" s="2" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
@@ -2266,6 +2754,9 @@
       <c r="C67" t="s">
         <v>259</v>
       </c>
+      <c r="D67" s="2" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
@@ -2277,6 +2768,9 @@
       <c r="C68" t="s">
         <v>256</v>
       </c>
+      <c r="D68" s="2" t="s">
+        <v>377</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
@@ -2288,6 +2782,9 @@
       <c r="C69" t="s">
         <v>260</v>
       </c>
+      <c r="D69" s="2" t="s">
+        <v>428</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
@@ -2338,6 +2835,9 @@
       <c r="C73" t="s">
         <v>256</v>
       </c>
+      <c r="D73" s="2" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
@@ -2349,6 +2849,9 @@
       <c r="C74" t="s">
         <v>256</v>
       </c>
+      <c r="D74" s="2" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
@@ -2360,6 +2863,9 @@
       <c r="C75" t="s">
         <v>256</v>
       </c>
+      <c r="D75" s="2" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
@@ -2371,6 +2877,9 @@
       <c r="C76" t="s">
         <v>249</v>
       </c>
+      <c r="D76" s="2" t="s">
+        <v>424</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
@@ -2396,6 +2905,9 @@
       <c r="C78" t="s">
         <v>266</v>
       </c>
+      <c r="D78" s="2" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
@@ -2407,6 +2919,9 @@
       <c r="C79" t="s">
         <v>259</v>
       </c>
+      <c r="D79" s="2" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
@@ -2432,6 +2947,9 @@
       <c r="C81" t="s">
         <v>256</v>
       </c>
+      <c r="D81" s="2" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
@@ -2443,6 +2961,9 @@
       <c r="C82" t="s">
         <v>266</v>
       </c>
+      <c r="D82" s="2" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
@@ -2454,6 +2975,9 @@
       <c r="C83" t="s">
         <v>270</v>
       </c>
+      <c r="D83" s="2" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
@@ -2479,6 +3003,9 @@
       <c r="C85" t="s">
         <v>260</v>
       </c>
+      <c r="D85" s="2" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
@@ -2504,6 +3031,9 @@
       <c r="C87" t="s">
         <v>256</v>
       </c>
+      <c r="D87" s="2" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
@@ -2565,6 +3095,9 @@
       <c r="C92" t="s">
         <v>249</v>
       </c>
+      <c r="D92" s="2" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
@@ -2576,6 +3109,9 @@
       <c r="C93" t="s">
         <v>256</v>
       </c>
+      <c r="D93" s="2" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
@@ -2587,6 +3123,9 @@
       <c r="C94" t="s">
         <v>255</v>
       </c>
+      <c r="D94" s="2" t="s">
+        <v>434</v>
+      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
@@ -2620,6 +3159,9 @@
       <c r="C97" t="s">
         <v>271</v>
       </c>
+      <c r="D97" s="2" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
@@ -2645,6 +3187,9 @@
       <c r="C99" t="s">
         <v>256</v>
       </c>
+      <c r="D99" s="2" t="s">
+        <v>417</v>
+      </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
@@ -2678,6 +3223,9 @@
       <c r="C102" t="s">
         <v>256</v>
       </c>
+      <c r="D102" s="2" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
@@ -2689,6 +3237,9 @@
       <c r="C103" t="s">
         <v>249</v>
       </c>
+      <c r="D103" s="2" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
@@ -2700,6 +3251,9 @@
       <c r="C104" t="s">
         <v>256</v>
       </c>
+      <c r="D104" s="2" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
@@ -2711,6 +3265,9 @@
       <c r="C105" t="s">
         <v>271</v>
       </c>
+      <c r="D105" s="2" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
@@ -2750,6 +3307,9 @@
       <c r="C108" t="s">
         <v>271</v>
       </c>
+      <c r="D108" s="2" t="s">
+        <v>368</v>
+      </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
@@ -2772,6 +3332,9 @@
       <c r="C110" t="s">
         <v>256</v>
       </c>
+      <c r="D110" s="2" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
@@ -2783,6 +3346,9 @@
       <c r="C111" t="s">
         <v>260</v>
       </c>
+      <c r="D111" s="2" t="s">
+        <v>436</v>
+      </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
@@ -2808,6 +3374,9 @@
       <c r="C113" t="s">
         <v>257</v>
       </c>
+      <c r="D113" s="2" t="s">
+        <v>375</v>
+      </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
@@ -2819,6 +3388,9 @@
       <c r="C114" t="s">
         <v>251</v>
       </c>
+      <c r="D114" s="2" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
@@ -2830,6 +3402,9 @@
       <c r="C115" t="s">
         <v>256</v>
       </c>
+      <c r="D115" s="2" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
@@ -2880,6 +3455,9 @@
       <c r="C119" t="s">
         <v>267</v>
       </c>
+      <c r="D119" s="2" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
@@ -2891,6 +3469,9 @@
       <c r="C120" t="s">
         <v>268</v>
       </c>
+      <c r="D120" s="2" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
@@ -2902,6 +3483,9 @@
       <c r="C121" t="s">
         <v>256</v>
       </c>
+      <c r="D121" s="2" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
@@ -2913,6 +3497,9 @@
       <c r="C122" t="s">
         <v>251</v>
       </c>
+      <c r="D122" s="2" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
@@ -2949,6 +3536,9 @@
       <c r="C125" t="s">
         <v>250</v>
       </c>
+      <c r="D125" s="2" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
@@ -2960,6 +3550,9 @@
       <c r="C126" t="s">
         <v>249</v>
       </c>
+      <c r="D126" s="2" t="s">
+        <v>440</v>
+      </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
@@ -2971,6 +3564,9 @@
       <c r="C127" t="s">
         <v>256</v>
       </c>
+      <c r="D127" s="2" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
@@ -3010,6 +3606,9 @@
       <c r="C130" t="s">
         <v>251</v>
       </c>
+      <c r="D130" s="2" t="s">
+        <v>411</v>
+      </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
@@ -3021,6 +3620,9 @@
       <c r="C131" t="s">
         <v>251</v>
       </c>
+      <c r="D131" s="2" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
@@ -3032,6 +3634,9 @@
       <c r="C132" t="s">
         <v>272</v>
       </c>
+      <c r="D132" s="2" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
@@ -3057,6 +3662,9 @@
       <c r="C134" t="s">
         <v>250</v>
       </c>
+      <c r="D134" s="2" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
@@ -3082,6 +3690,9 @@
       <c r="C136" t="s">
         <v>250</v>
       </c>
+      <c r="D136" s="2" t="s">
+        <v>426</v>
+      </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
@@ -3107,6 +3718,9 @@
       <c r="C138" t="s">
         <v>256</v>
       </c>
+      <c r="D138" s="2" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
@@ -3132,6 +3746,9 @@
       <c r="C140" t="s">
         <v>270</v>
       </c>
+      <c r="D140" s="2" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
@@ -3143,6 +3760,9 @@
       <c r="C141" t="s">
         <v>256</v>
       </c>
+      <c r="D141" s="2" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
@@ -3179,6 +3799,9 @@
       <c r="C144" t="s">
         <v>251</v>
       </c>
+      <c r="D144" s="2" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
@@ -3190,6 +3813,9 @@
       <c r="C145" t="s">
         <v>250</v>
       </c>
+      <c r="D145" s="2" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
@@ -3212,6 +3838,9 @@
       <c r="C147" t="s">
         <v>249</v>
       </c>
+      <c r="D147" s="2" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
@@ -3223,6 +3852,9 @@
       <c r="C148" t="s">
         <v>250</v>
       </c>
+      <c r="D148" s="2" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
@@ -3262,6 +3894,9 @@
       <c r="C151" t="s">
         <v>266</v>
       </c>
+      <c r="D151" s="2" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
@@ -3273,6 +3908,9 @@
       <c r="C152" t="s">
         <v>256</v>
       </c>
+      <c r="D152" s="2" t="s">
+        <v>450</v>
+      </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
@@ -3284,6 +3922,9 @@
       <c r="C153" t="s">
         <v>251</v>
       </c>
+      <c r="D153" s="2" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
@@ -3295,6 +3936,9 @@
       <c r="C154" t="s">
         <v>256</v>
       </c>
+      <c r="D154" s="2" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
@@ -3306,6 +3950,9 @@
       <c r="C155" t="s">
         <v>250</v>
       </c>
+      <c r="D155" s="2" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
@@ -3317,6 +3964,9 @@
       <c r="C156" t="s">
         <v>250</v>
       </c>
+      <c r="D156" s="2" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
@@ -3353,6 +4003,9 @@
       <c r="C159" t="s">
         <v>271</v>
       </c>
+      <c r="D159" s="2" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
@@ -3364,6 +4017,9 @@
       <c r="C160" t="s">
         <v>256</v>
       </c>
+      <c r="D160" s="2" t="s">
+        <v>409</v>
+      </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
@@ -3389,6 +4045,9 @@
       <c r="C162" t="s">
         <v>261</v>
       </c>
+      <c r="D162" s="2" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
@@ -3414,6 +4073,9 @@
       <c r="C164" t="s">
         <v>271</v>
       </c>
+      <c r="D164" s="2" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
@@ -3436,6 +4098,9 @@
       <c r="C166" t="s">
         <v>256</v>
       </c>
+      <c r="D166" s="2" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
@@ -3497,6 +4162,9 @@
       <c r="C171" t="s">
         <v>251</v>
       </c>
+      <c r="D171" s="2" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
@@ -3508,6 +4176,9 @@
       <c r="C172" t="s">
         <v>250</v>
       </c>
+      <c r="D172" s="2" t="s">
+        <v>360</v>
+      </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
@@ -3519,6 +4190,9 @@
       <c r="C173" t="s">
         <v>271</v>
       </c>
+      <c r="D173" s="2" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
@@ -3530,6 +4204,9 @@
       <c r="C174" t="s">
         <v>256</v>
       </c>
+      <c r="D174" s="2" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
@@ -3541,6 +4218,9 @@
       <c r="C175" t="s">
         <v>256</v>
       </c>
+      <c r="D175" s="2" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
@@ -3552,6 +4232,9 @@
       <c r="C176" t="s">
         <v>256</v>
       </c>
+      <c r="D176" s="2" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
@@ -3602,6 +4285,9 @@
       <c r="C180" t="s">
         <v>272</v>
       </c>
+      <c r="D180" s="2" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
@@ -3641,6 +4327,9 @@
       <c r="C183" t="s">
         <v>260</v>
       </c>
+      <c r="D183" s="2" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
@@ -3652,6 +4341,9 @@
       <c r="C184" t="s">
         <v>266</v>
       </c>
+      <c r="D184" s="2" t="s">
+        <v>431</v>
+      </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
@@ -3663,6 +4355,9 @@
       <c r="C185" t="s">
         <v>263</v>
       </c>
+      <c r="D185" s="2" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
@@ -3702,6 +4397,9 @@
       <c r="C188" t="s">
         <v>256</v>
       </c>
+      <c r="D188" s="2" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
@@ -3713,6 +4411,9 @@
       <c r="C189" t="s">
         <v>263</v>
       </c>
+      <c r="D189" s="2" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
@@ -3735,6 +4436,9 @@
       <c r="C191" t="s">
         <v>256</v>
       </c>
+      <c r="D191" s="2" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
@@ -3760,6 +4464,9 @@
       <c r="C193" t="s">
         <v>271</v>
       </c>
+      <c r="D193" s="2" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
@@ -3782,6 +4489,9 @@
       <c r="C195" t="s">
         <v>272</v>
       </c>
+      <c r="D195" s="2" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
@@ -3835,6 +4545,9 @@
       <c r="C199" t="s">
         <v>256</v>
       </c>
+      <c r="D199" s="2" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
@@ -3857,6 +4570,9 @@
       <c r="C201" t="s">
         <v>268</v>
       </c>
+      <c r="D201" s="2" t="s">
+        <v>439</v>
+      </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
@@ -3882,6 +4598,9 @@
       <c r="C203" t="s">
         <v>256</v>
       </c>
+      <c r="D203" s="2" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
@@ -3893,6 +4612,9 @@
       <c r="C204" t="s">
         <v>256</v>
       </c>
+      <c r="D204" s="2" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
@@ -3915,6 +4637,9 @@
       <c r="C206" t="s">
         <v>260</v>
       </c>
+      <c r="D206" s="2" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
@@ -3940,6 +4665,9 @@
       <c r="C208" t="s">
         <v>264</v>
       </c>
+      <c r="D208" s="2" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
@@ -3951,6 +4679,9 @@
       <c r="C209" t="s">
         <v>256</v>
       </c>
+      <c r="D209" s="2" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
@@ -3962,6 +4693,9 @@
       <c r="C210" t="s">
         <v>260</v>
       </c>
+      <c r="D210" s="2" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
@@ -3973,6 +4707,9 @@
       <c r="C211" t="s">
         <v>250</v>
       </c>
+      <c r="D211" s="2" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
@@ -3984,6 +4721,9 @@
       <c r="C212" t="s">
         <v>256</v>
       </c>
+      <c r="D212" s="2" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
@@ -4009,6 +4749,9 @@
       <c r="C214" t="s">
         <v>256</v>
       </c>
+      <c r="D214" s="2" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
@@ -4020,6 +4763,9 @@
       <c r="C215" t="s">
         <v>256</v>
       </c>
+      <c r="D215" s="2" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
@@ -4031,6 +4777,9 @@
       <c r="C216" t="s">
         <v>264</v>
       </c>
+      <c r="D216" s="2" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
@@ -4053,6 +4802,9 @@
       <c r="C218" t="s">
         <v>251</v>
       </c>
+      <c r="D218" s="2" t="s">
+        <v>371</v>
+      </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
@@ -4064,6 +4816,9 @@
       <c r="C219" t="s">
         <v>249</v>
       </c>
+      <c r="D219" s="2" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
@@ -4075,6 +4830,9 @@
       <c r="C220" t="s">
         <v>256</v>
       </c>
+      <c r="D220" s="2" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
@@ -4086,6 +4844,9 @@
       <c r="C221" t="s">
         <v>265</v>
       </c>
+      <c r="D221" s="2" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
@@ -4147,6 +4908,9 @@
       <c r="C226" t="s">
         <v>256</v>
       </c>
+      <c r="D226" s="2" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
@@ -4172,6 +4936,9 @@
       <c r="C228" t="s">
         <v>256</v>
       </c>
+      <c r="D228" s="2" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
@@ -4183,6 +4950,9 @@
       <c r="C229" t="s">
         <v>256</v>
       </c>
+      <c r="D229" s="2" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
@@ -4194,6 +4964,9 @@
       <c r="C230" t="s">
         <v>271</v>
       </c>
+      <c r="D230" s="2" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
@@ -4205,6 +4978,9 @@
       <c r="C231" t="s">
         <v>262</v>
       </c>
+      <c r="D231" s="2" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
@@ -4230,6 +5006,9 @@
       <c r="C233" t="s">
         <v>262</v>
       </c>
+      <c r="D233" s="2" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
@@ -4241,6 +5020,9 @@
       <c r="C234" t="s">
         <v>251</v>
       </c>
+      <c r="D234" s="2" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
@@ -4252,6 +5034,9 @@
       <c r="C235" t="s">
         <v>266</v>
       </c>
+      <c r="D235" s="2" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
@@ -4263,6 +5048,9 @@
       <c r="C236" t="s">
         <v>260</v>
       </c>
+      <c r="D236" s="2" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
@@ -4288,6 +5076,9 @@
       <c r="C238" t="s">
         <v>251</v>
       </c>
+      <c r="D238" s="2" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
@@ -4299,6 +5090,9 @@
       <c r="C239" t="s">
         <v>257</v>
       </c>
+      <c r="D239" s="2" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
@@ -4310,6 +5104,9 @@
       <c r="C240" t="s">
         <v>256</v>
       </c>
+      <c r="D240" s="2" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
@@ -4321,6 +5118,9 @@
       <c r="C241" t="s">
         <v>251</v>
       </c>
+      <c r="D241" s="2" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
@@ -4332,6 +5132,9 @@
       <c r="C242" t="s">
         <v>256</v>
       </c>
+      <c r="D242" s="2" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
@@ -4343,6 +5146,9 @@
       <c r="C243" t="s">
         <v>271</v>
       </c>
+      <c r="D243" s="2" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
@@ -4378,6 +5184,9 @@
       </c>
       <c r="C246" t="s">
         <v>250</v>
+      </c>
+      <c r="D246" s="2" t="s">
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -4454,6 +5263,146 @@
     <hyperlink ref="D192" r:id="rId70" location="get-firefox-plugins" xr:uid="{DC647779-FF8E-1F44-AEC9-F7292AE76238}"/>
     <hyperlink ref="D139" r:id="rId71" location="get-firefox-plugins" xr:uid="{2C7A65B5-5C13-E847-9E84-53ADA79491AD}"/>
     <hyperlink ref="D207" r:id="rId72" location="get-firefox-plugins" xr:uid="{81831373-774D-524D-A69F-960A2577CA23}"/>
+    <hyperlink ref="D39" r:id="rId73" location="get-last-remote-action-performance" xr:uid="{E109A40A-6A3A-EF4B-B3D0-10D4D732119A}"/>
+    <hyperlink ref="D242" r:id="rId74" location="install-windows-update" xr:uid="{40C89325-E5D1-D747-B803-189234DC4A9B}"/>
+    <hyperlink ref="D212" r:id="rId75" location="get-last-feature-update-status" xr:uid="{FDDE4B50-EB95-A34E-9042-D3CD0D60161D}"/>
+    <hyperlink ref="D147" r:id="rId76" location="get-windows-feature-update-diagnosis" xr:uid="{E555D429-DDEC-774A-A3E3-6D9F5EACD947}"/>
+    <hyperlink ref="D57" r:id="rId77" location="invoke-windows-update" xr:uid="{BCC25EFC-7E88-3646-98D1-D08E05DF51DE}"/>
+    <hyperlink ref="D233" r:id="rId78" location="get-battery-status" xr:uid="{96D30A2A-11B1-D945-B385-EC86C579468A}"/>
+    <hyperlink ref="D104" r:id="rId79" location="set-power-plan" xr:uid="{98814183-1010-294F-B79C-9885FBC1B669}"/>
+    <hyperlink ref="D56" r:id="rId80" location="get-user-folder-size" xr:uid="{EABFBD27-9B39-4843-8FED-C14B453FA0AD}"/>
+    <hyperlink ref="D23" r:id="rId81" location="get-power-plan" xr:uid="{5D47F9F7-AC26-5D4B-832D-16B6F6CCAD79}"/>
+    <hyperlink ref="D203" r:id="rId82" location="get-consumption-information" xr:uid="{A137A088-26BB-F84C-9CE9-F6AFD6736BE4}"/>
+    <hyperlink ref="D26" r:id="rId83" location="get-network-drives" xr:uid="{1B5627AC-B4DA-294B-B146-F0B0973A55BC}"/>
+    <hyperlink ref="D125" r:id="rId84" location="map-network-drive" xr:uid="{DF10CB53-22A2-EB4F-964B-94221BE097F0}"/>
+    <hyperlink ref="D27" r:id="rId85" location="get-device-azure-ad-status" xr:uid="{23CC2C40-75EE-0044-8FAA-C2A8353E9C33}"/>
+    <hyperlink ref="D220" r:id="rId86" location="get-secure-boot-status" xr:uid="{E8D507BD-2BBB-2040-9A9F-A737BCEAAB67}"/>
+    <hyperlink ref="D28" r:id="rId87" location="get-directx-information" xr:uid="{04E0DE17-2D87-184D-9B80-C66028842053}"/>
+    <hyperlink ref="D238" r:id="rId88" location="get-bitlocker-information" xr:uid="{9A4CFDD1-CB50-B441-9AB1-D179EF7EE122}"/>
+    <hyperlink ref="D156" r:id="rId89" location="get-network-configuration" xr:uid="{5E61D15C-9699-824C-9CD5-1C41BCFBCF7C}"/>
+    <hyperlink ref="D172" r:id="rId90" location="get-wi-fi-information" xr:uid="{2C27DC74-C0AC-A440-AB41-2D3E70C25F22}"/>
+    <hyperlink ref="D148" r:id="rId91" location="test-connection-from-device" xr:uid="{631BFA18-E1AF-414E-8516-787E431C250C}"/>
+    <hyperlink ref="D63" r:id="rId92" location="clear-dns-cache" xr:uid="{388EDD62-176C-9640-885B-2E2A306F7B7F}"/>
+    <hyperlink ref="D211" r:id="rId93" location="get-interface-connection-status" xr:uid="{C413537C-239E-774D-AB86-AB5363B2518D}"/>
+    <hyperlink ref="D246" r:id="rId94" location="get-active-ip-address" xr:uid="{16A3F26C-1FD6-B941-8458-E5C5FD8108A6}"/>
+    <hyperlink ref="D159" r:id="rId95" location="get-microsoft-edge-plugins" xr:uid="{0886C504-4C8E-B545-B204-71345A8F05F1}"/>
+    <hyperlink ref="D32" r:id="rId96" location="set-microsoft-edge-plugins" xr:uid="{5B28EA8E-8F82-5945-A47F-21BEA1A35669}"/>
+    <hyperlink ref="D230" r:id="rId97" location="clear-microsoft-edge-settings" xr:uid="{564751A7-EADD-4E4F-B55A-4351A2CDE585}"/>
+    <hyperlink ref="D108" r:id="rId98" location="clear-internet-explorer-11-settings" xr:uid="{C496FAB0-AAA1-2D4C-B836-6DFA549416DC}"/>
+    <hyperlink ref="D173" r:id="rId99" location="get-internet-explorer-plugins" xr:uid="{BFCA0F5A-EEA3-1340-B216-C872187DB3F4}"/>
+    <hyperlink ref="D193" r:id="rId100" location="set-internet-explorer-plugins" xr:uid="{EED356BE-DB42-2643-9A81-A915D3EBF2A9}"/>
+    <hyperlink ref="D218" r:id="rId101" location="start-officescan-location-scan" xr:uid="{BCE562FE-AD90-C440-A7C9-B5C2CFD839FC}"/>
+    <hyperlink ref="D30" r:id="rId102" location="update-officescan-definition" xr:uid="{2D66A3D2-A439-D045-AED7-CC717243E5CE}"/>
+    <hyperlink ref="D239" r:id="rId103" location="reinstall-jamf" xr:uid="{08C5695C-E175-874B-BB25-8F717BC5ABF4}"/>
+    <hyperlink ref="D43" r:id="rId104" location="get-jamf-agent-status" xr:uid="{03C404DC-A5C7-924C-A8F2-10460A2D5CE8}"/>
+    <hyperlink ref="D113" r:id="rId105" location="invoke-jamf-reconnect" xr:uid="{F91C5926-D046-7B4F-A6FE-A46E5E13441F}"/>
+    <hyperlink ref="D25" r:id="rId106" location="get-startup-impact" xr:uid="{75356258-43F7-F045-9A24-6863506B80BF}"/>
+    <hyperlink ref="D68" r:id="rId107" location="disable-application-from-startup-menu" xr:uid="{E8C5FDE4-187C-384B-B8D2-C0906FB4568B}"/>
+    <hyperlink ref="D121" r:id="rId108" location="get-gpo-startup-impact" xr:uid="{0C1BF9E9-31E6-5A4B-8EAC-97F53C2EB202}"/>
+    <hyperlink ref="D236" r:id="rId109" location="disk-cleanup" xr:uid="{731F56FC-9257-DB4D-80D6-3E1790E58A4E}"/>
+    <hyperlink ref="D183" r:id="rId110" location="system-cleanup" xr:uid="{4B14D7C0-C727-1643-A7D7-C626FCEA1792}"/>
+    <hyperlink ref="D79" r:id="rId111" location="request-vpn-connection-for-compliance" xr:uid="{4E222C6E-09CA-7740-AE92-3637B472C09A}"/>
+    <hyperlink ref="D47" r:id="rId112" location="update-group-policy-settings" xr:uid="{BD556A1A-AC6F-DA40-A30D-62048F97C871}"/>
+    <hyperlink ref="D215" r:id="rId113" location="get-hardware-and-bios-information" xr:uid="{D1B116E0-8B84-864A-9B91-4B67E2285094}"/>
+    <hyperlink ref="D188" r:id="rId114" location="reset-print-spooler" xr:uid="{BE22777E-8569-A94C-B6BD-ADD7DB66E7A3}"/>
+    <hyperlink ref="D185" r:id="rId115" location="skype-for-business-diagnostics" xr:uid="{93F7C390-B303-6445-9454-AFD3A413794F}"/>
+    <hyperlink ref="D21" r:id="rId116" location="get-windows-information" xr:uid="{421D706E-7F01-F947-8A2A-7C5AD5A66E1D}"/>
+    <hyperlink ref="D171" r:id="rId117" location="get-accounts-information" xr:uid="{C3443823-3A47-2945-9BD2-BE0955F0D76A}"/>
+    <hyperlink ref="D102" r:id="rId118" location="get-auto-login-status" xr:uid="{1FDBA3C0-E9EB-CB44-90EE-7AE905860FFA}"/>
+    <hyperlink ref="D110" r:id="rId119" location="get-automatic-updates-status" xr:uid="{84B22EFA-610C-9A4C-AB21-5AD0D2C23564}"/>
+    <hyperlink ref="D114" r:id="rId120" location="get-encryption-information" xr:uid="{0EABEEC4-C53E-E44E-A417-FA0B64077128}"/>
+    <hyperlink ref="D240" r:id="rId121" location="get-firewall-options" xr:uid="{2508BAA5-40B6-B646-9FD7-C4C6A3102F55}"/>
+    <hyperlink ref="D73" r:id="rId122" location="get-xprotect-status" xr:uid="{B705AB19-E197-754B-BE34-B606510413A9}"/>
+    <hyperlink ref="D226" r:id="rId123" location="invoke-log-off-for-windows" xr:uid="{ADF9DFDC-6885-D14D-BEAB-4AE43E1D02AE}"/>
+    <hyperlink ref="D61" r:id="rId124" location="invoke-shut-down-for-windows" xr:uid="{7D2DAFB0-0981-A34B-83DC-88C5FD84D355}"/>
+    <hyperlink ref="D81" r:id="rId125" location="restart-windows-device" xr:uid="{BA206258-BA80-E640-AE72-57DF58429083}"/>
+    <hyperlink ref="D62" r:id="rId126" location="invoke-log-off-for-macos" xr:uid="{93448484-5228-F14A-B991-390BC4539AC5}"/>
+    <hyperlink ref="D174" r:id="rId127" location="invoke-shut-down-for-macos" xr:uid="{724A8647-039C-954F-B727-2FF4F20DC554}"/>
+    <hyperlink ref="D31" r:id="rId128" location="restart-macos-device" xr:uid="{EEF3380C-1689-804E-B9C8-13FA5A6AEC02}"/>
+    <hyperlink ref="D115" r:id="rId129" location="restart-service" xr:uid="{F4C2ECBB-35C9-3145-BB2B-8113D542045C}"/>
+    <hyperlink ref="D66" r:id="rId130" location="get-service-information" xr:uid="{D76055FB-A10E-E246-87A7-72B53467ED9E}"/>
+    <hyperlink ref="D87" r:id="rId131" location="set-service-information" xr:uid="{84CD7F6F-BB3F-1D44-9B3B-FDA5DAEA5B74}"/>
+    <hyperlink ref="D191" r:id="rId132" location="hosts-file-integrity-check" xr:uid="{42F69D08-84F6-0E40-95E8-D6270FBB5BD8}"/>
+    <hyperlink ref="D134" r:id="rId133" location="get-smb1-status" xr:uid="{271BDF70-B7D0-B44B-A95A-81EA23EC4719}"/>
+    <hyperlink ref="D29" r:id="rId134" location="disable-smb1" xr:uid="{63AAF72F-9DFE-B643-AD10-221ED2A88E75}"/>
+    <hyperlink ref="D122" r:id="rId135" location="remove-certificates" xr:uid="{15810CCA-3CD9-FD40-A038-0B1F7D6C3666}"/>
+    <hyperlink ref="D144" r:id="rId136" location="trusted-root-certification-authorities-certificate-store-integrity-check" xr:uid="{7DC912E3-8C9E-ED4A-BB9A-265C167630F1}"/>
+    <hyperlink ref="D36" r:id="rId137" location="get-windows-security-center-health-status" xr:uid="{36D1FC44-1710-A74B-AC0C-2352EAC99138}"/>
+    <hyperlink ref="D93" r:id="rId138" location="get-windows-registry-key-values" xr:uid="{6EDDC99C-52DE-314D-BCEA-0B02C59A4FD7}"/>
+    <hyperlink ref="D160" r:id="rId139" location="set-windows-registry-key-value" xr:uid="{12D3243F-DD09-4A4E-B637-D896CF4A89D3}"/>
+    <hyperlink ref="D59" r:id="rId140" location="get-windows-defender-information" xr:uid="{B6AF7CFA-20E3-EF44-A117-BBC0A8FE853A}"/>
+    <hyperlink ref="D130" r:id="rId141" location="update-windows-defender-definition" xr:uid="{D40CAAA7-D838-6E42-B136-A86500278382}"/>
+    <hyperlink ref="D241" r:id="rId142" location="set-windows-defender-scheduled-scan" xr:uid="{E2CBF0D2-B695-9843-82F1-EBED6E9EF60D}"/>
+    <hyperlink ref="D44" r:id="rId143" location="start-windows-defender-scan" xr:uid="{31A92EAA-561E-E143-8D46-76AB559CE8AE}"/>
+    <hyperlink ref="D83" r:id="rId144" location="uninstall-microsoft-office-visio-and-project" xr:uid="{81925D7F-6E01-4B42-8368-D5394400D27C}"/>
+    <hyperlink ref="D35" r:id="rId145" location="uninstall-adobe-dc-professional" xr:uid="{D371492B-5066-B548-B6A4-4AF88F17A631}"/>
+    <hyperlink ref="D51" r:id="rId146" location="get-local-administrators" xr:uid="{C53AB4F9-F197-1746-8723-2B0FFE1197C2}"/>
+    <hyperlink ref="D99" r:id="rId147" location="enable-user-access-control" xr:uid="{BE9F35F5-DBD8-3941-B781-59C287E3213F}"/>
+    <hyperlink ref="D15" r:id="rId148" location="get-vmware-optimization-information" xr:uid="{D4664AF0-DB0E-FC44-9CC6-8108A028F837}"/>
+    <hyperlink ref="D13" r:id="rId149" location="invoke-sccm-upgrade-to-windows-11" xr:uid="{AAFB5638-5EB2-AC42-82A3-7F6D36BF296F}"/>
+    <hyperlink ref="D38" r:id="rId150" location="get-geolocation" xr:uid="{214F7D8D-14F4-9E46-A6E0-F3F2543D0DD9}"/>
+    <hyperlink ref="D45" r:id="rId151" location="kerberos-password-expiration-reminder" xr:uid="{3C768303-4FAC-6D4E-BC61-CDD1A97714A4}"/>
+    <hyperlink ref="D46" r:id="rId152" location="get-virtual-apps-session-response-time" xr:uid="{17A85F33-289F-304E-988E-1DAA085C0620}"/>
+    <hyperlink ref="D48" r:id="rId153" location="remove-credentials-from-credential-manager" xr:uid="{E81C55D1-13B6-8946-8BF6-4BDCE21D7D68}"/>
+    <hyperlink ref="D52" r:id="rId154" location="get-event-log" xr:uid="{80B77BC0-1534-2F41-945B-5595FE903332}"/>
+    <hyperlink ref="D76" r:id="rId155" location="get-number-of-log-events" xr:uid="{9E0C96BD-4CC2-2B4B-B5EC-E5E218DDC7B5}"/>
+    <hyperlink ref="D54" r:id="rId156" location="get-onedrive-status" xr:uid="{9CA7101F-E129-A14B-940C-297D078A0155}"/>
+    <hyperlink ref="D60" r:id="rId157" location="get-computer-assigned-group-policy" xr:uid="{C3FD084A-0C70-4544-86E7-AB1307D471EB}"/>
+    <hyperlink ref="D136" r:id="rId158" location="test-domain-connection" xr:uid="{B364AD30-6B91-8B4F-886B-8D53A5459A9E}"/>
+    <hyperlink ref="D67" r:id="rId159" location="check-anyconnect-timeout" xr:uid="{3721BB6C-B3F3-0246-9C5C-99331340C96D}"/>
+    <hyperlink ref="D69" r:id="rId160" location="get-disk-health" xr:uid="{C96067F9-482B-F94C-9025-DB6EB0C851B8}"/>
+    <hyperlink ref="D74" r:id="rId161" location="get-frameworks-version" xr:uid="{482C2210-2C39-B64F-9462-F10EF2DECE61}"/>
+    <hyperlink ref="D75" r:id="rId162" location="get-performance-monitor-data" xr:uid="{8D438758-EE3E-AD4F-A064-BE71E393A53C}"/>
+    <hyperlink ref="D78" r:id="rId163" location="enable-tray-accessibility" xr:uid="{C5B9A353-E72A-9E4D-A205-9BD05048BD3A}"/>
+    <hyperlink ref="D82" r:id="rId164" location="enable-tray-accessibility" xr:uid="{50820CD3-BAE9-0241-BB9C-2CEECABA1FAF}"/>
+    <hyperlink ref="D85" r:id="rId165" location="get-physical-disks-information" xr:uid="{F3CA3CE0-2B76-0C40-B52A-19E963F27413}"/>
+    <hyperlink ref="D92" r:id="rId166" location="get-apple-unified-logging" xr:uid="{5D75FA7B-1D9D-BA4A-84BD-ECE3579CB3C5}"/>
+    <hyperlink ref="D94" r:id="rId167" location="get-onedrive-information" xr:uid="{D9E3DC65-0786-0840-AF7D-D89E3012EE85}"/>
+    <hyperlink ref="D97" r:id="rId168" location="get-chrome-plugins" xr:uid="{E8DE2CA7-9434-134A-8F51-FD52D170FBF6}"/>
+    <hyperlink ref="D103" r:id="rId169" location="read-mini-dump" xr:uid="{10D97AB6-260E-4347-859A-301D3FEE4D0D}"/>
+    <hyperlink ref="D105" r:id="rId170" location="test-chrome-plugins-compliance" xr:uid="{673FF6E7-E650-F844-858D-2F7702CE7D7B}"/>
+    <hyperlink ref="D111" r:id="rId171" location="clear-recycle-bin" xr:uid="{F35A5149-A2C3-6D41-BC2B-28B2B7502982}"/>
+    <hyperlink ref="D119" r:id="rId172" location="get-azure-virtual-desktop-information" xr:uid="{0923476D-7DF1-304D-8051-1ECAEFC48561}"/>
+    <hyperlink ref="D120" r:id="rId173" location="get-mcafee-agent-status" xr:uid="{3785E506-F0B9-B14B-989D-A494535EA947}"/>
+    <hyperlink ref="D201" r:id="rId174" location="update-mcafee-agent-policy" xr:uid="{9DAE4096-5388-4644-B55F-86C8B1ACD2A9}"/>
+    <hyperlink ref="D126" r:id="rId175" location="get-failed-logins" xr:uid="{C218E354-1C68-7F44-879B-33CE2277E676}"/>
+    <hyperlink ref="D127" r:id="rId176" location="get-configuration-drift" xr:uid="{C9D913C4-6869-9243-8DCC-E8C7EAA89FD7}"/>
+    <hyperlink ref="D131" r:id="rId177" location="mitigate-cve20191552" xr:uid="{832A5AF5-96CF-EE48-9181-6D32817CCE02}"/>
+    <hyperlink ref="D132" r:id="rId178" location="get-citrix-vdi-connection-details" xr:uid="{2D2558BA-D52F-3A4F-BAD3-F01561219535}"/>
+    <hyperlink ref="D138" r:id="rId179" location="get-powershell-information" xr:uid="{0751676D-FA31-0647-B224-21F340774A2F}"/>
+    <hyperlink ref="D140" r:id="rId180" location="update-winrar" xr:uid="{AB0AFA9B-2452-D747-B30E-7E85A2291102}"/>
+    <hyperlink ref="D141" r:id="rId181" location="invoke-proactive-password-reset" xr:uid="{F1DEDF0A-5C52-CE4C-9F8C-0BD742456640}"/>
+    <hyperlink ref="D145" r:id="rId182" location="disable-device-network-isolation" xr:uid="{05B56905-94CE-4F4B-B2B0-ECF45FAC0DA0}"/>
+    <hyperlink ref="D155" r:id="rId183" location="enable-device-network-isolation" xr:uid="{1F683CD3-B61C-CD4F-A4BC-0819C6D46D6F}"/>
+    <hyperlink ref="D151" r:id="rId184" location="set-application-experience" xr:uid="{83BAA126-7E1F-6D44-B427-46234D591772}"/>
+    <hyperlink ref="D152" r:id="rId185" location="get-device-manager-information" xr:uid="{2D5F65DF-5CC8-A542-A690-FDCB7685389C}"/>
+    <hyperlink ref="D175" r:id="rId186" location="get-folder-size" xr:uid="{FA539233-9A8D-D74A-977B-DF79FEFF75C5}"/>
+    <hyperlink ref="D166" r:id="rId187" location="get-windows-experience-index" xr:uid="{EC2B9D00-DC0A-664C-8876-AD4EFB5947A6}"/>
+    <hyperlink ref="D153" r:id="rId188" location="enable-bitlocker-encryption" xr:uid="{48A9D60B-38EC-B747-8963-E456EB52B4D7}"/>
+    <hyperlink ref="D154" r:id="rId189" location="get-device-hardware-id" xr:uid="{EB1CF790-79C8-A246-B6D2-41EB17859704}"/>
+    <hyperlink ref="D162" r:id="rId190" location="start-application-or-task-sequence" xr:uid="{5918C150-7ACD-B64F-BD06-E6D439D51B6D}"/>
+    <hyperlink ref="D208" r:id="rId191" location="repair-wmi" xr:uid="{A2EFD61F-2755-684D-9E4A-E1EF14555E40}"/>
+    <hyperlink ref="D164" r:id="rId192" location="get-chrome-plugins" xr:uid="{77777AFA-6D0F-CE40-BBE3-07A80AE8F542}"/>
+    <hyperlink ref="D176" r:id="rId193" location="get-boot-details" xr:uid="{4E3A5FDE-D2F0-7E40-BA6B-0777BCFF21AA}"/>
+    <hyperlink ref="D180" r:id="rId194" location="get-citrix-information" xr:uid="{C574DB2D-8F08-9E4D-B955-0EBEC362BE68}"/>
+    <hyperlink ref="D184" r:id="rId195" location="enable-tray-accessibility" xr:uid="{113E8D42-5F76-0F45-BDE0-045400DCE22D}"/>
+    <hyperlink ref="D189" r:id="rId196" location="get-skype-last-call" xr:uid="{83D8C3BB-B1A1-FE45-A1C3-1C33FFE2081C}"/>
+    <hyperlink ref="D219" r:id="rId197" location="copy-skype-log-files" xr:uid="{E5290D09-D30C-C647-8D8E-086B8A98C06A}"/>
+    <hyperlink ref="D195" r:id="rId198" location="get-citrix-session-client-versions" xr:uid="{5B4118B9-C22F-4544-9B20-AE16672FE55A}"/>
+    <hyperlink ref="D199" r:id="rId199" location="set-boot-autologger" xr:uid="{44762418-45BE-554C-9BEC-1B51ABD9D865}"/>
+    <hyperlink ref="D204" r:id="rId200" location="set-usb-storage-access" xr:uid="{CBEFDB75-32D0-4A4D-9DDF-CBFAE4562594}"/>
+    <hyperlink ref="D206" r:id="rId201" location="get-old-files-size" xr:uid="{6B7FA8E8-7A39-0C41-9F50-682FA9EE0226}"/>
+    <hyperlink ref="D209" r:id="rId202" location="get-windows-disk-configuration" xr:uid="{0FECA4FD-F3A5-904A-BC2B-418C6AA73B78}"/>
+    <hyperlink ref="D210" r:id="rId203" location="get-file-extension-total-size" xr:uid="{3A2E09C3-6983-7B44-BDA3-E851C2EDC9A6}"/>
+    <hyperlink ref="D214" r:id="rId204" location="get-plist-file-settings" xr:uid="{4C041A7A-7984-9B41-8CC6-6A68BFBAEF6B}"/>
+    <hyperlink ref="D216" r:id="rId205" location="get-wmi-data" xr:uid="{F3B34BDF-CB67-B54B-9175-137367113BD2}"/>
+    <hyperlink ref="D221" r:id="rId206" location="get-microsoft-intune-device-status" xr:uid="{453F5C77-8598-BD43-B005-00878AB4E7CA}"/>
+    <hyperlink ref="D228" r:id="rId207" location="get-warranty-information" xr:uid="{7B63C9F4-CEF0-FB4C-B6CE-62BE84DEC5DD}"/>
+    <hyperlink ref="D229" r:id="rId208" location="get-usb-audio-device-information" xr:uid="{0F12B012-536B-9547-9CA5-1D9FEBD0B24B}"/>
+    <hyperlink ref="D231" r:id="rId209" location="get-multiple-batteries-status" xr:uid="{2ACB9CCD-B52B-C84C-9CF4-BD45CF818F96}"/>
+    <hyperlink ref="D234" r:id="rId210" location="check-certificate-validity" xr:uid="{E15A562C-9D3E-094E-89BE-4F127F35B4E4}"/>
+    <hyperlink ref="D235" r:id="rId211" location="get-application-experience-browser-extension-status" xr:uid="{BFD3CD56-081F-E740-A4B4-0594153861F3}"/>
+    <hyperlink ref="D243" r:id="rId212" location="get-firefox-plugins" xr:uid="{29F2B42A-2D4F-A74E-9DC7-BABC9423F8A1}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Code refinement and documentation
</commit_message>
<xml_diff>
--- a/categories.xlsx
+++ b/categories.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toufikswar/Documents/dev/waitress-salesforce/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tswar/Documents/Python/waitress-salesforce/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B277A2FE-9B24-454F-9CAB-A80F834B278A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C613E3-EE79-064E-AB28-5529C329322D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-10620" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_remote_actions" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_remote_actions!$A$1:$D$246</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all_remote_actions!$A$1:$E$253</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="488">
   <si>
     <t>Name</t>
   </si>
@@ -1460,6 +1460,45 @@
   </si>
   <si>
     <t>https://www.nexthink.com/library/get-application-experience-browser-extension-status/#get-application-experience-browser-extension-status</t>
+  </si>
+  <si>
+    <t>Clear Recycle Bin macOS</t>
+  </si>
+  <si>
+    <t>Set Firewall Options</t>
+  </si>
+  <si>
+    <t>Get File Extension Total Size macOS</t>
+  </si>
+  <si>
+    <t>Disk Cleanup macOS</t>
+  </si>
+  <si>
+    <t>Get Old Files Size macOS</t>
+  </si>
+  <si>
+    <t>Clear Trash Bin macOS</t>
+  </si>
+  <si>
+    <t>Remove Auto Login</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/disk-cleanup-for-macos/#clear-trash-bin-macos</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/disk-cleanup-for-macos/#get-file-extension-total-size-macos</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/disk-cleanup-for-macos/#disk-cleanup-macos</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/disk-cleanup-for-macos/#get-old-files-size-macos</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>https://www.nexthink.com/library/macos-ensure-compliance-state/</t>
   </si>
 </sst>
 </file>
@@ -1834,10 +1873,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D246"/>
+  <dimension ref="A1:E253"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1845,9 +1884,10 @@
     <col min="2" max="2" width="54.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="108.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1857,8 +1897,11 @@
       <c r="D1" s="1" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1868,8 +1911,11 @@
       <c r="C2" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1882,8 +1928,11 @@
       <c r="D3" s="2" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1896,8 +1945,11 @@
       <c r="D4" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1910,8 +1962,11 @@
       <c r="D5" s="2" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1921,8 +1976,11 @@
       <c r="C6" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1935,8 +1993,11 @@
       <c r="D7" s="2" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1949,8 +2010,11 @@
       <c r="D8" s="2" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1960,8 +2024,11 @@
       <c r="C9" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1974,8 +2041,11 @@
       <c r="D10" s="2" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1988,8 +2058,11 @@
       <c r="D11" s="2" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2002,8 +2075,11 @@
       <c r="D12" s="2" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2016,8 +2092,11 @@
       <c r="D13" s="2" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2030,8 +2109,11 @@
       <c r="D14" s="2" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2044,8 +2126,11 @@
       <c r="D15" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2058,8 +2143,11 @@
       <c r="D16" s="2" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2072,8 +2160,11 @@
       <c r="D17" s="2" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2086,8 +2177,11 @@
       <c r="D18" s="2" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2100,8 +2194,11 @@
       <c r="D19" s="2" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2114,8 +2211,11 @@
       <c r="D20" s="2" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2128,8 +2228,11 @@
       <c r="D21" s="2" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2142,8 +2245,11 @@
       <c r="D22" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2156,8 +2262,11 @@
       <c r="D23" s="2" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2167,8 +2276,11 @@
       <c r="C24" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2181,8 +2293,11 @@
       <c r="D25" s="2" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2195,8 +2310,11 @@
       <c r="D26" s="2" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2209,8 +2327,11 @@
       <c r="D27" s="2" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2223,8 +2344,11 @@
       <c r="D28" s="2" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2237,8 +2361,11 @@
       <c r="D29" s="2" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2251,8 +2378,11 @@
       <c r="D30" s="2" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2265,8 +2395,11 @@
       <c r="D31" s="2" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2279,8 +2412,11 @@
       <c r="D32" s="2" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2290,8 +2426,11 @@
       <c r="C33" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2304,8 +2443,11 @@
       <c r="D34" s="2" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2318,8 +2460,11 @@
       <c r="D35" s="2" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2332,8 +2477,11 @@
       <c r="D36" s="2" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2346,8 +2494,11 @@
       <c r="D37" s="2" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2360,8 +2511,11 @@
       <c r="D38" s="2" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2374,8 +2528,11 @@
       <c r="D39" s="2" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2388,8 +2545,11 @@
       <c r="D40" s="2" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2402,8 +2562,11 @@
       <c r="D41" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2413,8 +2576,11 @@
       <c r="C42" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2427,8 +2593,11 @@
       <c r="D43" s="2" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2441,8 +2610,11 @@
       <c r="D44" s="2" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2455,8 +2627,11 @@
       <c r="D45" s="2" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2469,8 +2644,11 @@
       <c r="D46" s="2" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2483,8 +2661,11 @@
       <c r="D47" s="2" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2497,8 +2678,11 @@
       <c r="D48" s="2" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2511,8 +2695,11 @@
       <c r="D49" s="2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2522,8 +2709,11 @@
       <c r="C50" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2536,8 +2726,11 @@
       <c r="D51" s="2" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2550,8 +2743,11 @@
       <c r="D52" s="2" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2564,8 +2760,11 @@
       <c r="D53" s="2" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2578,8 +2777,11 @@
       <c r="D54" s="2" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2589,8 +2791,11 @@
       <c r="C55" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2603,8 +2808,11 @@
       <c r="D56" s="2" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2617,8 +2825,11 @@
       <c r="D57" s="2" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2631,8 +2842,11 @@
       <c r="D58" s="2" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2645,8 +2859,11 @@
       <c r="D59" s="2" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2659,8 +2876,11 @@
       <c r="D60" s="2" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2673,8 +2893,11 @@
       <c r="D61" s="2" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2687,8 +2910,11 @@
       <c r="D62" s="2" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2701,8 +2927,11 @@
       <c r="D63" s="2" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2715,8 +2944,11 @@
       <c r="D64" s="2" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2729,8 +2961,11 @@
       <c r="D65" s="2" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2743,8 +2978,11 @@
       <c r="D66" s="2" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2757,8 +2995,11 @@
       <c r="D67" s="2" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2771,8 +3012,11 @@
       <c r="D68" s="2" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2785,8 +3029,11 @@
       <c r="D69" s="2" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2796,8 +3043,11 @@
       <c r="C70" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2810,8 +3060,11 @@
       <c r="D71" s="2" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2824,8 +3077,11 @@
       <c r="D72" s="2" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2838,8 +3094,11 @@
       <c r="D73" s="2" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2852,8 +3111,11 @@
       <c r="D74" s="2" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2866,8 +3128,11 @@
       <c r="D75" s="2" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2880,8 +3145,11 @@
       <c r="D76" s="2" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2894,8 +3162,11 @@
       <c r="D77" s="2" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2908,8 +3179,11 @@
       <c r="D78" s="2" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2922,8 +3196,11 @@
       <c r="D79" s="2" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2936,8 +3213,11 @@
       <c r="D80" s="2" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2950,8 +3230,11 @@
       <c r="D81" s="2" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2964,8 +3247,11 @@
       <c r="D82" s="2" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2978,8 +3264,11 @@
       <c r="D83" s="2" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2992,8 +3281,11 @@
       <c r="D84" s="2" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3006,8 +3298,11 @@
       <c r="D85" s="2" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3020,8 +3315,11 @@
       <c r="D86" s="2" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3034,8 +3332,11 @@
       <c r="D87" s="2" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3048,8 +3349,11 @@
       <c r="D88" s="2" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3059,8 +3363,11 @@
       <c r="C89" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3073,8 +3380,11 @@
       <c r="D90" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3084,8 +3394,11 @@
       <c r="C91" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3098,8 +3411,11 @@
       <c r="D92" s="2" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3112,8 +3428,11 @@
       <c r="D93" s="2" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3126,8 +3445,11 @@
       <c r="D94" s="2" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3137,8 +3459,11 @@
       <c r="C95" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3148,8 +3473,11 @@
       <c r="C96" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3162,8 +3490,11 @@
       <c r="D97" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3176,8 +3507,11 @@
       <c r="D98" s="2" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3190,8 +3524,11 @@
       <c r="D99" s="2" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3201,8 +3538,11 @@
       <c r="C100" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3212,8 +3552,11 @@
       <c r="C101" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3226,8 +3569,11 @@
       <c r="D102" s="2" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3240,8 +3586,11 @@
       <c r="D103" s="2" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3254,8 +3603,11 @@
       <c r="D104" s="2" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -3268,8 +3620,11 @@
       <c r="D105" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -3282,8 +3637,11 @@
       <c r="D106" s="2" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -3296,8 +3654,11 @@
       <c r="D107" s="2" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3310,8 +3671,11 @@
       <c r="D108" s="2" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3321,8 +3685,11 @@
       <c r="C109" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3335,8 +3702,11 @@
       <c r="D110" s="2" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -3349,8 +3719,11 @@
       <c r="D111" s="2" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -3363,8 +3736,11 @@
       <c r="D112" s="2" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -3377,8 +3753,11 @@
       <c r="D113" s="2" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -3391,8 +3770,11 @@
       <c r="D114" s="2" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -3405,8 +3787,11 @@
       <c r="D115" s="2" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -3416,8 +3801,11 @@
       <c r="C116" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -3430,8 +3818,11 @@
       <c r="D117" s="2" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -3444,8 +3835,11 @@
       <c r="D118" s="2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -3458,8 +3852,11 @@
       <c r="D119" s="2" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -3472,8 +3869,11 @@
       <c r="D120" s="2" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -3486,8 +3886,11 @@
       <c r="D121" s="2" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -3500,8 +3903,11 @@
       <c r="D122" s="2" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -3514,8 +3920,11 @@
       <c r="D123" s="2" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -3525,8 +3934,11 @@
       <c r="C124" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -3539,8 +3951,11 @@
       <c r="D125" s="2" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -3553,8 +3968,11 @@
       <c r="D126" s="2" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -3567,8 +3985,11 @@
       <c r="D127" s="2" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -3581,8 +4002,11 @@
       <c r="D128" s="2" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -3595,8 +4019,11 @@
       <c r="D129" s="2" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -3609,8 +4036,11 @@
       <c r="D130" s="2" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -3623,8 +4053,11 @@
       <c r="D131" s="2" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -3637,8 +4070,11 @@
       <c r="D132" s="2" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -3651,8 +4087,11 @@
       <c r="D133" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -3665,8 +4104,11 @@
       <c r="D134" s="2" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -3679,8 +4121,11 @@
       <c r="D135" s="2" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -3693,8 +4138,11 @@
       <c r="D136" s="2" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -3707,8 +4155,11 @@
       <c r="D137" s="2" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -3721,8 +4172,11 @@
       <c r="D138" s="2" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -3735,8 +4189,11 @@
       <c r="D139" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -3749,8 +4206,11 @@
       <c r="D140" s="2" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E140">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -3763,8 +4223,11 @@
       <c r="D141" s="2" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -3774,8 +4237,11 @@
       <c r="C142" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -3788,8 +4254,11 @@
       <c r="D143" s="2" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -3802,8 +4271,11 @@
       <c r="D144" s="2" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -3816,8 +4288,11 @@
       <c r="D145" s="2" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -3827,8 +4302,11 @@
       <c r="C146" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -3841,8 +4319,11 @@
       <c r="D147" s="2" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -3855,8 +4336,11 @@
       <c r="D148" s="2" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -3869,8 +4353,11 @@
       <c r="D149" s="2" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -3883,8 +4370,11 @@
       <c r="D150" s="2" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -3897,8 +4387,11 @@
       <c r="D151" s="2" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -3911,8 +4404,11 @@
       <c r="D152" s="2" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -3925,8 +4421,11 @@
       <c r="D153" s="2" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -3939,8 +4438,11 @@
       <c r="D154" s="2" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -3953,8 +4455,11 @@
       <c r="D155" s="2" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -3967,8 +4472,11 @@
       <c r="D156" s="2" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -3981,8 +4489,11 @@
       <c r="D157" s="2" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -3992,8 +4503,11 @@
       <c r="C158" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -4006,8 +4520,11 @@
       <c r="D159" s="2" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -4020,8 +4537,11 @@
       <c r="D160" s="2" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -4034,8 +4554,11 @@
       <c r="D161" s="2" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -4048,8 +4571,11 @@
       <c r="D162" s="2" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -4062,8 +4588,11 @@
       <c r="D163" s="2" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -4076,8 +4605,11 @@
       <c r="D164" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -4087,8 +4619,11 @@
       <c r="C165" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -4101,8 +4636,11 @@
       <c r="D166" s="2" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -4115,8 +4653,11 @@
       <c r="D167" s="2" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -4126,8 +4667,11 @@
       <c r="C168" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -4137,8 +4681,11 @@
       <c r="C169" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -4151,8 +4698,11 @@
       <c r="D170" s="2" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -4165,8 +4715,11 @@
       <c r="D171" s="2" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -4179,8 +4732,11 @@
       <c r="D172" s="2" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -4193,8 +4749,11 @@
       <c r="D173" s="2" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -4207,8 +4766,11 @@
       <c r="D174" s="2" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -4221,8 +4783,11 @@
       <c r="D175" s="2" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -4235,8 +4800,11 @@
       <c r="D176" s="2" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -4246,8 +4814,11 @@
       <c r="C177" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -4260,8 +4831,11 @@
       <c r="D178" s="2" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -4274,8 +4848,11 @@
       <c r="D179" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -4288,8 +4865,11 @@
       <c r="D180" s="2" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -4302,8 +4882,11 @@
       <c r="D181" s="2" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -4316,8 +4899,11 @@
       <c r="D182" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -4330,8 +4916,11 @@
       <c r="D183" s="2" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -4344,8 +4933,11 @@
       <c r="D184" s="2" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -4358,8 +4950,11 @@
       <c r="D185" s="2" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -4372,8 +4967,11 @@
       <c r="D186" s="2" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -4386,8 +4984,11 @@
       <c r="D187" s="2" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -4400,8 +5001,11 @@
       <c r="D188" s="2" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -4414,8 +5018,11 @@
       <c r="D189" s="2" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E189">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -4425,8 +5032,11 @@
       <c r="C190" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -4439,8 +5049,11 @@
       <c r="D191" s="2" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -4453,8 +5066,11 @@
       <c r="D192" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -4467,8 +5083,11 @@
       <c r="D193" s="2" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -4478,8 +5097,11 @@
       <c r="C194" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -4492,8 +5114,11 @@
       <c r="D195" s="2" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -4506,8 +5131,11 @@
       <c r="D196" s="2" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -4520,8 +5148,11 @@
       <c r="D197" s="2" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -4534,8 +5165,11 @@
       <c r="D198" s="2" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -4548,8 +5182,11 @@
       <c r="D199" s="2" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -4559,8 +5196,11 @@
       <c r="C200" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -4573,8 +5213,11 @@
       <c r="D201" s="2" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -4587,8 +5230,11 @@
       <c r="D202" s="2" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -4601,8 +5247,11 @@
       <c r="D203" s="2" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -4615,8 +5264,11 @@
       <c r="D204" s="2" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -4626,8 +5278,11 @@
       <c r="C205" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -4640,8 +5295,11 @@
       <c r="D206" s="2" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -4654,8 +5312,11 @@
       <c r="D207" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -4668,8 +5329,11 @@
       <c r="D208" s="2" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -4682,8 +5346,11 @@
       <c r="D209" s="2" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -4696,8 +5363,11 @@
       <c r="D210" s="2" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -4710,8 +5380,11 @@
       <c r="D211" s="2" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -4724,8 +5397,11 @@
       <c r="D212" s="2" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -4738,8 +5414,11 @@
       <c r="D213" s="2" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -4752,8 +5431,11 @@
       <c r="D214" s="2" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -4766,8 +5448,11 @@
       <c r="D215" s="2" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -4780,8 +5465,11 @@
       <c r="D216" s="2" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -4791,8 +5479,11 @@
       <c r="C217" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -4805,8 +5496,11 @@
       <c r="D218" s="2" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -4819,8 +5513,11 @@
       <c r="D219" s="2" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -4833,8 +5530,11 @@
       <c r="D220" s="2" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -4847,8 +5547,11 @@
       <c r="D221" s="2" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -4861,8 +5564,11 @@
       <c r="D222" s="2" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -4872,8 +5578,11 @@
       <c r="C223" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -4883,8 +5592,11 @@
       <c r="C224" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -4897,8 +5609,11 @@
       <c r="D225" s="2" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -4911,8 +5626,11 @@
       <c r="D226" s="2" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -4925,8 +5643,11 @@
       <c r="D227" s="2" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -4939,8 +5660,11 @@
       <c r="D228" s="2" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -4953,8 +5677,11 @@
       <c r="D229" s="2" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -4967,8 +5694,11 @@
       <c r="D230" s="2" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -4981,8 +5711,11 @@
       <c r="D231" s="2" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -4995,8 +5728,11 @@
       <c r="D232" s="2" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -5009,8 +5745,11 @@
       <c r="D233" s="2" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -5023,8 +5762,11 @@
       <c r="D234" s="2" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -5037,8 +5779,11 @@
       <c r="D235" s="2" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -5051,8 +5796,11 @@
       <c r="D236" s="2" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -5065,8 +5813,11 @@
       <c r="D237" s="2" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -5079,8 +5830,11 @@
       <c r="D238" s="2" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -5093,8 +5847,11 @@
       <c r="D239" s="2" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -5107,8 +5864,11 @@
       <c r="D240" s="2" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -5121,8 +5881,11 @@
       <c r="D241" s="2" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -5135,8 +5898,11 @@
       <c r="D242" s="2" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -5149,8 +5915,11 @@
       <c r="D243" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -5160,8 +5929,11 @@
       <c r="C244" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -5174,8 +5946,11 @@
       <c r="D245" s="2" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E245">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -5187,6 +5962,128 @@
       </c>
       <c r="D246" s="2" t="s">
         <v>364</v>
+      </c>
+      <c r="E246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A247" s="1">
+        <v>245</v>
+      </c>
+      <c r="B247" t="s">
+        <v>475</v>
+      </c>
+      <c r="C247" t="s">
+        <v>260</v>
+      </c>
+      <c r="D247" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="E247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A248" s="1">
+        <v>246</v>
+      </c>
+      <c r="B248" t="s">
+        <v>476</v>
+      </c>
+      <c r="C248" t="s">
+        <v>251</v>
+      </c>
+      <c r="D248" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="E248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A249" s="1">
+        <v>247</v>
+      </c>
+      <c r="B249" t="s">
+        <v>477</v>
+      </c>
+      <c r="C249" t="s">
+        <v>260</v>
+      </c>
+      <c r="D249" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="E249">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A250" s="1">
+        <v>248</v>
+      </c>
+      <c r="B250" t="s">
+        <v>478</v>
+      </c>
+      <c r="C250" t="s">
+        <v>260</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="E250">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A251" s="1">
+        <v>249</v>
+      </c>
+      <c r="B251" t="s">
+        <v>479</v>
+      </c>
+      <c r="C251" t="s">
+        <v>260</v>
+      </c>
+      <c r="D251" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="E251">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A252" s="1">
+        <v>250</v>
+      </c>
+      <c r="B252" t="s">
+        <v>480</v>
+      </c>
+      <c r="C252" t="s">
+        <v>260</v>
+      </c>
+      <c r="D252" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="E252">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A253" s="1">
+        <v>251</v>
+      </c>
+      <c r="B253" t="s">
+        <v>481</v>
+      </c>
+      <c r="C253" t="s">
+        <v>251</v>
+      </c>
+      <c r="D253" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="E253">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5403,6 +6300,13 @@
     <hyperlink ref="D234" r:id="rId210" location="check-certificate-validity" xr:uid="{E15A562C-9D3E-094E-89BE-4F127F35B4E4}"/>
     <hyperlink ref="D235" r:id="rId211" location="get-application-experience-browser-extension-status" xr:uid="{BFD3CD56-081F-E740-A4B4-0594153861F3}"/>
     <hyperlink ref="D243" r:id="rId212" location="get-firefox-plugins" xr:uid="{29F2B42A-2D4F-A74E-9DC7-BABC9423F8A1}"/>
+    <hyperlink ref="D247" r:id="rId213" location="clear-trash-bin-macos" xr:uid="{27EE5A2C-F318-EC41-B977-484C179AC056}"/>
+    <hyperlink ref="D249" r:id="rId214" location="get-file-extension-total-size-macos" xr:uid="{0DD97418-567B-A74E-8333-349A1FD978C0}"/>
+    <hyperlink ref="D250" r:id="rId215" location="disk-cleanup-macos" xr:uid="{D9B13388-EA39-D240-BC60-BB719973FA34}"/>
+    <hyperlink ref="D251" r:id="rId216" location="get-old-files-size-macos" xr:uid="{430A5DBC-7063-D74B-BCD8-B9ED96C002E4}"/>
+    <hyperlink ref="D252" r:id="rId217" location="clear-trash-bin-macos" xr:uid="{382F5CDF-EC85-884F-B195-815335FAD6EB}"/>
+    <hyperlink ref="D248" r:id="rId218" xr:uid="{47A92A79-57C3-FA47-9FB6-B08DEA6E81E8}"/>
+    <hyperlink ref="D253" r:id="rId219" xr:uid="{16E2333A-11AD-E740-A7EA-9C31E86EB792}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>